<commit_message>
Force mass balance to zero if flow and initial concentration of organism biomass are both zero
</commit_message>
<xml_diff>
--- a/COM-dFBA/Scripts/paramTables.xlsx
+++ b/COM-dFBA/Scripts/paramTables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zorrilla\Desktop\COM-dFBA\Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{3FA97F8F-C43E-4892-B529-C2EF08B2C542}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A0D76B7D-7D31-49DE-986B-448CED432177}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="20475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="20475" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vmax" sheetId="1" r:id="rId1"/>
@@ -936,10 +936,10 @@
     <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="142">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1141,7 +1141,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1193,7 +1193,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1397,7 +1397,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M41" sqref="M41"/>
     </sheetView>
   </sheetViews>
@@ -5315,8 +5315,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5331,7 +5331,7 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
         <v>19</v>
@@ -5349,7 +5349,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>22.2901960784314</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -5374,7 +5374,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>43.043137254902</v>
+        <v>0</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -5399,7 +5399,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1.3333333333333299</v>
+        <v>0</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -5445,7 +5445,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="35">
-        <v>6.55</v>
+        <v>0</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -5493,7 +5493,7 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="38">
+      <c r="A8" s="37">
         <v>10</v>
       </c>
       <c r="B8" s="17">
@@ -5519,7 +5519,7 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="38">
+      <c r="A9" s="37">
         <v>20</v>
       </c>
       <c r="B9" s="17">
@@ -5544,7 +5544,7 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="38">
+      <c r="A10" s="37">
         <v>4.4710000000000001</v>
       </c>
       <c r="B10" s="17">
@@ -5570,7 +5570,7 @@
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="38">
+      <c r="A11" s="37">
         <v>1.4079999999999999</v>
       </c>
       <c r="B11" s="35">
@@ -5596,7 +5596,7 @@
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="38">
+      <c r="A12" s="37">
         <v>3.4910000000000001</v>
       </c>
       <c r="B12" s="17">
@@ -5623,7 +5623,7 @@
       <c r="L12" s="22"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="38">
+      <c r="A13" s="37">
         <v>2.2120000000000002</v>
       </c>
       <c r="B13" s="17">
@@ -5650,7 +5650,7 @@
       <c r="L13" s="22"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="38">
+      <c r="A14" s="37">
         <v>3.4609999999999999</v>
       </c>
       <c r="B14" s="17">
@@ -5677,7 +5677,7 @@
       <c r="L14" s="22"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="38">
+      <c r="A15" s="37">
         <v>2.7629999999999999</v>
       </c>
       <c r="B15" s="17">
@@ -5704,7 +5704,7 @@
       <c r="L15" s="22"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="38">
+      <c r="A16" s="37">
         <v>0.47199999999999998</v>
       </c>
       <c r="B16" s="17">
@@ -5731,7 +5731,7 @@
       <c r="L16" s="22"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="38">
+      <c r="A17" s="37">
         <v>1.2589999999999999</v>
       </c>
       <c r="B17" s="17">
@@ -5758,7 +5758,7 @@
       <c r="L17" s="22"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="38">
+      <c r="A18" s="37">
         <v>5.0979999999999999</v>
       </c>
       <c r="B18" s="17">
@@ -5785,7 +5785,7 @@
       <c r="L18" s="22"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="38">
+      <c r="A19" s="37">
         <v>2.734</v>
       </c>
       <c r="B19" s="35">
@@ -6179,10 +6179,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="38" t="s">
         <v>122</v>
       </c>
-      <c r="D1" s="37"/>
+      <c r="D1" s="38"/>
       <c r="E1" s="4"/>
       <c r="G1" s="4"/>
       <c r="P1" t="s">

</xml_diff>